<commit_message>
Add gender field and employee #
closes #419
</commit_message>
<xml_diff>
--- a/public/assets/documents/census-template.xlsx
+++ b/public/assets/documents/census-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petersonbrock/Documents/GitHub/Granite/granite/public/assets/documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jeremy/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DEC4463-8E8B-1C49-B8D9-FBE8BF330475}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1ABD6B2-980D-5D41-9ACA-B9B834700DEF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41140" yWindow="1840" windowWidth="28040" windowHeight="17440" xr2:uid="{97D58E43-8915-7943-952A-C87060369A36}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14020" xr2:uid="{97D58E43-8915-7943-952A-C87060369A36}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>First Name</t>
   </si>
@@ -103,6 +103,12 @@
   </si>
   <si>
     <t>Workers Comp Class Code</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Employee Number</t>
   </si>
 </sst>
 </file>
@@ -138,8 +144,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11DA4282-F3AA-0D4B-984E-19A12D8C3155}">
-  <dimension ref="A1:Z1"/>
+  <dimension ref="A1:AB2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -465,28 +472,30 @@
     <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8" customWidth="1"/>
-    <col min="19" max="19" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="27" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
+    <col min="6" max="7" width="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.33203125" customWidth="1"/>
+    <col min="16" max="16" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8" customWidth="1"/>
+    <col min="21" max="21" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="27" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="22.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -500,71 +509,80 @@
         <v>5</v>
       </c>
       <c r="E1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>12</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>16</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>2</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P1" t="s">
         <v>17</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>18</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>25</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>3</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>24</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>21</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>22</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>23</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>13</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>14</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>15</v>
       </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="K2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>